<commit_message>
Improved tests 1 and 3
Exported eucl distances, added variant level forecasts for test3
</commit_message>
<xml_diff>
--- a/test3_graphs/fitted_data_set.xlsx
+++ b/test3_graphs/fitted_data_set.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="125">
   <si>
     <t>Division</t>
   </si>
@@ -391,6 +391,9 @@
   </si>
   <si>
     <t>No. Weeks</t>
+  </si>
+  <si>
+    <t>Variant level</t>
   </si>
 </sst>
 </file>
@@ -398,10 +401,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -429,10 +440,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,11 +725,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DH30"/>
+  <dimension ref="A1:DH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <pane xSplit="6" topLeftCell="CQ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CW27" sqref="CW27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +741,7 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="93" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="96" max="112" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10777,7 +10789,1444 @@
         <v>43.314149352412599</v>
       </c>
     </row>
+    <row r="31" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="CQ31" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="CR32" s="2">
+        <v>-0.99999999999997202</v>
+      </c>
+      <c r="CS32" s="2">
+        <v>51.999999999999901</v>
+      </c>
+      <c r="CT32" s="2">
+        <v>181</v>
+      </c>
+      <c r="CU32" s="2">
+        <v>233</v>
+      </c>
+      <c r="CV32" s="2">
+        <v>204</v>
+      </c>
+      <c r="CW32" s="2">
+        <v>163</v>
+      </c>
+      <c r="CX32" s="2">
+        <v>133</v>
+      </c>
+      <c r="CY32" s="2">
+        <v>80.999999999999901</v>
+      </c>
+      <c r="CZ32" s="2">
+        <v>7.0000000000000098</v>
+      </c>
+      <c r="DA32" s="2">
+        <v>70.999999999999702</v>
+      </c>
+      <c r="DB32" s="2">
+        <v>463</v>
+      </c>
+      <c r="DC32" s="2">
+        <v>542</v>
+      </c>
+      <c r="DD32" s="2">
+        <v>416</v>
+      </c>
+      <c r="DE32" s="2">
+        <v>144</v>
+      </c>
+      <c r="DF32" s="2">
+        <v>85.999999999999801</v>
+      </c>
+      <c r="DG32" s="2">
+        <v>176</v>
+      </c>
+      <c r="DH32" s="2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR33" s="2">
+        <v>4.9999999999999396</v>
+      </c>
+      <c r="CS33" s="2">
+        <v>-36.999999999999901</v>
+      </c>
+      <c r="CT33" s="2">
+        <v>-73.000000000000199</v>
+      </c>
+      <c r="CU33" s="2">
+        <v>-36</v>
+      </c>
+      <c r="CV33" s="2">
+        <v>29.999999999999901</v>
+      </c>
+      <c r="CW33" s="2">
+        <v>37</v>
+      </c>
+      <c r="CX33" s="2">
+        <v>78.999999999999901</v>
+      </c>
+      <c r="CY33" s="2">
+        <v>173</v>
+      </c>
+      <c r="CZ33" s="2">
+        <v>162</v>
+      </c>
+      <c r="DA33" s="2">
+        <v>210</v>
+      </c>
+      <c r="DB33" s="2">
+        <v>387</v>
+      </c>
+      <c r="DC33" s="2">
+        <v>485</v>
+      </c>
+      <c r="DD33" s="2">
+        <v>225</v>
+      </c>
+      <c r="DE33" s="2">
+        <v>33.999999999999901</v>
+      </c>
+      <c r="DF33" s="2">
+        <v>20.999999999999901</v>
+      </c>
+      <c r="DG33" s="2">
+        <v>-2.0000000000000702</v>
+      </c>
+      <c r="DH33" s="2">
+        <v>-37.000000000000099</v>
+      </c>
+    </row>
+    <row r="34" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR34" s="2">
+        <v>203.2</v>
+      </c>
+      <c r="CS34" s="2">
+        <v>196.2</v>
+      </c>
+      <c r="CT34" s="2">
+        <v>198.2</v>
+      </c>
+      <c r="CU34" s="2">
+        <v>206.2</v>
+      </c>
+      <c r="CV34" s="2">
+        <v>203.2</v>
+      </c>
+      <c r="CW34" s="2">
+        <v>200.2</v>
+      </c>
+      <c r="CX34" s="2">
+        <v>200.2</v>
+      </c>
+      <c r="CY34" s="2">
+        <v>208.2</v>
+      </c>
+      <c r="CZ34" s="2">
+        <v>209.2</v>
+      </c>
+      <c r="DA34" s="2">
+        <v>216.2</v>
+      </c>
+      <c r="DB34" s="2">
+        <v>214.2</v>
+      </c>
+      <c r="DC34" s="2">
+        <v>211.2</v>
+      </c>
+      <c r="DD34" s="2">
+        <v>207.2</v>
+      </c>
+      <c r="DE34" s="2">
+        <v>195.2</v>
+      </c>
+      <c r="DF34" s="2">
+        <v>191.2</v>
+      </c>
+      <c r="DG34" s="2">
+        <v>201.2</v>
+      </c>
+      <c r="DH34" s="2">
+        <v>194.2</v>
+      </c>
+    </row>
+    <row r="35" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR35" s="2">
+        <v>134.457142857143</v>
+      </c>
+      <c r="CS35" s="2">
+        <v>134.457142857143</v>
+      </c>
+      <c r="CT35" s="2">
+        <v>130.457142857143</v>
+      </c>
+      <c r="CU35" s="2">
+        <v>303.45714285714303</v>
+      </c>
+      <c r="CV35" s="2">
+        <v>186.457142857143</v>
+      </c>
+      <c r="CW35" s="2">
+        <v>214.457142857143</v>
+      </c>
+      <c r="CX35" s="2">
+        <v>274.45714285714303</v>
+      </c>
+      <c r="CY35" s="2">
+        <v>391.45714285714303</v>
+      </c>
+      <c r="CZ35" s="2">
+        <v>415.457142857142</v>
+      </c>
+      <c r="DA35" s="2">
+        <v>461.45714285714303</v>
+      </c>
+      <c r="DB35" s="2">
+        <v>615.45714285714303</v>
+      </c>
+      <c r="DC35" s="2">
+        <v>558.45714285714303</v>
+      </c>
+      <c r="DD35" s="2">
+        <v>263.45714285714303</v>
+      </c>
+      <c r="DE35" s="2">
+        <v>69.457142857142799</v>
+      </c>
+      <c r="DF35" s="2">
+        <v>65.457142857142799</v>
+      </c>
+      <c r="DG35" s="2">
+        <v>49.457142857142898</v>
+      </c>
+      <c r="DH35" s="2">
+        <v>74.457142857142799</v>
+      </c>
+    </row>
+    <row r="36" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR36" s="2">
+        <v>568.99999999999898</v>
+      </c>
+      <c r="CS36" s="2">
+        <v>565</v>
+      </c>
+      <c r="CT36" s="2">
+        <v>419.00000000000102</v>
+      </c>
+      <c r="CU36" s="2">
+        <v>821.00000000000205</v>
+      </c>
+      <c r="CV36" s="2">
+        <v>885.99999999999898</v>
+      </c>
+      <c r="CW36" s="2">
+        <v>1613</v>
+      </c>
+      <c r="CX36" s="2">
+        <v>1323</v>
+      </c>
+      <c r="CY36" s="2">
+        <v>2403</v>
+      </c>
+      <c r="CZ36" s="2">
+        <v>3139</v>
+      </c>
+      <c r="DA36" s="2">
+        <v>3846</v>
+      </c>
+      <c r="DB36" s="2">
+        <v>4305</v>
+      </c>
+      <c r="DC36" s="2">
+        <v>3505</v>
+      </c>
+      <c r="DD36" s="2">
+        <v>672.00000000000102</v>
+      </c>
+      <c r="DE36" s="2">
+        <v>224</v>
+      </c>
+      <c r="DF36" s="2">
+        <v>-337</v>
+      </c>
+      <c r="DG36" s="2">
+        <v>-300</v>
+      </c>
+      <c r="DH36" s="2">
+        <v>-339.00000000000102</v>
+      </c>
+    </row>
+    <row r="37" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR37" s="2">
+        <v>80.342857142857099</v>
+      </c>
+      <c r="CS37" s="2">
+        <v>82.342857142857099</v>
+      </c>
+      <c r="CT37" s="2">
+        <v>84.342857142857198</v>
+      </c>
+      <c r="CU37" s="2">
+        <v>97.342857142857198</v>
+      </c>
+      <c r="CV37" s="2">
+        <v>115.342857142857</v>
+      </c>
+      <c r="CW37" s="2">
+        <v>140.34285714285701</v>
+      </c>
+      <c r="CX37" s="2">
+        <v>91.342857142857198</v>
+      </c>
+      <c r="CY37" s="2">
+        <v>116.342857142857</v>
+      </c>
+      <c r="CZ37" s="2">
+        <v>93.342857142857099</v>
+      </c>
+      <c r="DA37" s="2">
+        <v>97.342857142857198</v>
+      </c>
+      <c r="DB37" s="2">
+        <v>91.342857142857099</v>
+      </c>
+      <c r="DC37" s="2">
+        <v>47.342857142857099</v>
+      </c>
+      <c r="DD37" s="2">
+        <v>20.342857142857099</v>
+      </c>
+      <c r="DE37" s="2">
+        <v>33.342857142857198</v>
+      </c>
+      <c r="DF37" s="2">
+        <v>39.342857142857198</v>
+      </c>
+      <c r="DG37" s="2">
+        <v>38.342857142857198</v>
+      </c>
+      <c r="DH37" s="2">
+        <v>41.342857142857099</v>
+      </c>
+    </row>
+    <row r="38" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR38" s="2">
+        <v>125.828571428571</v>
+      </c>
+      <c r="CS38" s="2">
+        <v>139.828571428571</v>
+      </c>
+      <c r="CT38" s="2">
+        <v>117.828571428571</v>
+      </c>
+      <c r="CU38" s="2">
+        <v>174.828571428571</v>
+      </c>
+      <c r="CV38" s="2">
+        <v>158.828571428571</v>
+      </c>
+      <c r="CW38" s="2">
+        <v>167.828571428571</v>
+      </c>
+      <c r="CX38" s="2">
+        <v>194.828571428571</v>
+      </c>
+      <c r="CY38" s="2">
+        <v>196.828571428571</v>
+      </c>
+      <c r="CZ38" s="2">
+        <v>126.828571428571</v>
+      </c>
+      <c r="DA38" s="2">
+        <v>75.828571428571394</v>
+      </c>
+      <c r="DB38" s="2">
+        <v>78.828571428571493</v>
+      </c>
+      <c r="DC38" s="2">
+        <v>146.828571428571</v>
+      </c>
+      <c r="DD38" s="2">
+        <v>153.828571428571</v>
+      </c>
+      <c r="DE38" s="2">
+        <v>100.828571428571</v>
+      </c>
+      <c r="DF38" s="2">
+        <v>113.828571428571</v>
+      </c>
+      <c r="DG38" s="2">
+        <v>128.828571428571</v>
+      </c>
+      <c r="DH38" s="2">
+        <v>116.828571428571</v>
+      </c>
+    </row>
+    <row r="39" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR39" s="2">
+        <v>3710.0285714285701</v>
+      </c>
+      <c r="CS39" s="2">
+        <v>4162.0285714285701</v>
+      </c>
+      <c r="CT39" s="2">
+        <v>4673.0285714285701</v>
+      </c>
+      <c r="CU39" s="2">
+        <v>5996.0285714285701</v>
+      </c>
+      <c r="CV39" s="2">
+        <v>5802.0285714285701</v>
+      </c>
+      <c r="CW39" s="2">
+        <v>6841.0285714285701</v>
+      </c>
+      <c r="CX39" s="2">
+        <v>7875.0285714285701</v>
+      </c>
+      <c r="CY39" s="2">
+        <v>11301.0285714286</v>
+      </c>
+      <c r="CZ39" s="2">
+        <v>11541.0285714286</v>
+      </c>
+      <c r="DA39" s="2">
+        <v>13437.0285714286</v>
+      </c>
+      <c r="DB39" s="2">
+        <v>18398.0285714286</v>
+      </c>
+      <c r="DC39" s="2">
+        <v>18622.0285714286</v>
+      </c>
+      <c r="DD39" s="2">
+        <v>5062.0285714285801</v>
+      </c>
+      <c r="DE39" s="2">
+        <v>2670.0285714285701</v>
+      </c>
+      <c r="DF39" s="2">
+        <v>2590.0285714285701</v>
+      </c>
+      <c r="DG39" s="2">
+        <v>2643.0285714285701</v>
+      </c>
+      <c r="DH39" s="2">
+        <v>2957.0285714285701</v>
+      </c>
+    </row>
+    <row r="40" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR40" s="2">
+        <v>1323.6571428571399</v>
+      </c>
+      <c r="CS40" s="2">
+        <v>1435.6571428571399</v>
+      </c>
+      <c r="CT40" s="2">
+        <v>1629.6571428571399</v>
+      </c>
+      <c r="CU40" s="2">
+        <v>1719.6571428571399</v>
+      </c>
+      <c r="CV40" s="2">
+        <v>1178.6571428571399</v>
+      </c>
+      <c r="CW40" s="2">
+        <v>1690.6571428571399</v>
+      </c>
+      <c r="CX40" s="2">
+        <v>1742.6571428571399</v>
+      </c>
+      <c r="CY40" s="2">
+        <v>2032.6571428571399</v>
+      </c>
+      <c r="CZ40" s="2">
+        <v>1552.6571428571399</v>
+      </c>
+      <c r="DA40" s="2">
+        <v>1851.6571428571399</v>
+      </c>
+      <c r="DB40" s="2">
+        <v>2529.6571428571401</v>
+      </c>
+      <c r="DC40" s="2">
+        <v>2134.6571428571401</v>
+      </c>
+      <c r="DD40" s="2">
+        <v>1224.6571428571399</v>
+      </c>
+      <c r="DE40" s="2">
+        <v>911.65714285714296</v>
+      </c>
+      <c r="DF40" s="2">
+        <v>1136.6571428571399</v>
+      </c>
+      <c r="DG40" s="2">
+        <v>1046.6571428571399</v>
+      </c>
+      <c r="DH40" s="2">
+        <v>799.65714285714296</v>
+      </c>
+    </row>
+    <row r="41" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR41" s="2">
+        <v>-32.657142857142702</v>
+      </c>
+      <c r="CS41" s="2">
+        <v>-50.657142857142802</v>
+      </c>
+      <c r="CT41" s="2">
+        <v>-66.657142857142702</v>
+      </c>
+      <c r="CU41" s="2">
+        <v>19.342857142857099</v>
+      </c>
+      <c r="CV41" s="2">
+        <v>-35.657142857142603</v>
+      </c>
+      <c r="CW41" s="2">
+        <v>-33.657142857142901</v>
+      </c>
+      <c r="CX41" s="2">
+        <v>14.3428571428572</v>
+      </c>
+      <c r="CY41" s="2">
+        <v>59.342857142857198</v>
+      </c>
+      <c r="CZ41" s="2">
+        <v>229.34285714285701</v>
+      </c>
+      <c r="DA41" s="2">
+        <v>278.34285714285699</v>
+      </c>
+      <c r="DB41" s="2">
+        <v>362.34285714285699</v>
+      </c>
+      <c r="DC41" s="2">
+        <v>186.34285714285701</v>
+      </c>
+      <c r="DD41" s="2">
+        <v>-58.657142857142702</v>
+      </c>
+      <c r="DE41" s="2">
+        <v>-104.657142857143</v>
+      </c>
+      <c r="DF41" s="2">
+        <v>-125.657142857143</v>
+      </c>
+      <c r="DG41" s="2">
+        <v>-128.65714285714299</v>
+      </c>
+      <c r="DH41" s="2">
+        <v>-130.65714285714299</v>
+      </c>
+    </row>
+    <row r="42" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR42" s="2">
+        <v>128.142857142857</v>
+      </c>
+      <c r="CS42" s="2">
+        <v>120.142857142857</v>
+      </c>
+      <c r="CT42" s="2">
+        <v>124.142857142857</v>
+      </c>
+      <c r="CU42" s="2">
+        <v>137.142857142857</v>
+      </c>
+      <c r="CV42" s="2">
+        <v>136.142857142857</v>
+      </c>
+      <c r="CW42" s="2">
+        <v>162.142857142857</v>
+      </c>
+      <c r="CX42" s="2">
+        <v>162.142857142857</v>
+      </c>
+      <c r="CY42" s="2">
+        <v>191.142857142857</v>
+      </c>
+      <c r="CZ42" s="2">
+        <v>197.142857142857</v>
+      </c>
+      <c r="DA42" s="2">
+        <v>188.142857142857</v>
+      </c>
+      <c r="DB42" s="2">
+        <v>189.142857142857</v>
+      </c>
+      <c r="DC42" s="2">
+        <v>232.142857142857</v>
+      </c>
+      <c r="DD42" s="2">
+        <v>205.142857142857</v>
+      </c>
+      <c r="DE42" s="2">
+        <v>148.142857142857</v>
+      </c>
+      <c r="DF42" s="2">
+        <v>142.142857142857</v>
+      </c>
+      <c r="DG42" s="2">
+        <v>142.142857142857</v>
+      </c>
+      <c r="DH42" s="2">
+        <v>141.142857142857</v>
+      </c>
+    </row>
+    <row r="43" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR43" s="2">
+        <v>380.17142857142801</v>
+      </c>
+      <c r="CS43" s="2">
+        <v>398.17142857142801</v>
+      </c>
+      <c r="CT43" s="2">
+        <v>412.17142857142898</v>
+      </c>
+      <c r="CU43" s="2">
+        <v>438.17142857142898</v>
+      </c>
+      <c r="CV43" s="2">
+        <v>548.17142857142801</v>
+      </c>
+      <c r="CW43" s="2">
+        <v>557.17142857142801</v>
+      </c>
+      <c r="CX43" s="2">
+        <v>574.17142857142903</v>
+      </c>
+      <c r="CY43" s="2">
+        <v>915.17142857142801</v>
+      </c>
+      <c r="CZ43" s="2">
+        <v>1049.1714285714299</v>
+      </c>
+      <c r="DA43" s="2">
+        <v>1233.1714285714299</v>
+      </c>
+      <c r="DB43" s="2">
+        <v>1347.1714285714299</v>
+      </c>
+      <c r="DC43" s="2">
+        <v>1246.1714285714299</v>
+      </c>
+      <c r="DD43" s="2">
+        <v>405.17142857142898</v>
+      </c>
+      <c r="DE43" s="2">
+        <v>331.17142857142801</v>
+      </c>
+      <c r="DF43" s="2">
+        <v>339.17142857142801</v>
+      </c>
+      <c r="DG43" s="2">
+        <v>331.17142857142898</v>
+      </c>
+      <c r="DH43" s="2">
+        <v>359.17142857142801</v>
+      </c>
+    </row>
+    <row r="44" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR44" s="2">
+        <v>192.17142857142801</v>
+      </c>
+      <c r="CS44" s="2">
+        <v>256.17142857142801</v>
+      </c>
+      <c r="CT44" s="2">
+        <v>336.17142857142898</v>
+      </c>
+      <c r="CU44" s="2">
+        <v>383.17142857143</v>
+      </c>
+      <c r="CV44" s="2">
+        <v>603.17142857142801</v>
+      </c>
+      <c r="CW44" s="2">
+        <v>669.17142857142903</v>
+      </c>
+      <c r="CX44" s="2">
+        <v>1406.1714285714299</v>
+      </c>
+      <c r="CY44" s="2">
+        <v>3205.1714285714302</v>
+      </c>
+      <c r="CZ44" s="2">
+        <v>3434.1714285714302</v>
+      </c>
+      <c r="DA44" s="2">
+        <v>2398.1714285714302</v>
+      </c>
+      <c r="DB44" s="2">
+        <v>2274.1714285714302</v>
+      </c>
+      <c r="DC44" s="2">
+        <v>1717.1714285714299</v>
+      </c>
+      <c r="DD44" s="2">
+        <v>334.17142857142801</v>
+      </c>
+      <c r="DE44" s="2">
+        <v>154.17142857142801</v>
+      </c>
+      <c r="DF44" s="2">
+        <v>116.171428571428</v>
+      </c>
+      <c r="DG44" s="2">
+        <v>133.171428571429</v>
+      </c>
+      <c r="DH44" s="2">
+        <v>131.17142857142801</v>
+      </c>
+    </row>
+    <row r="45" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR45" s="2">
+        <v>718.22857142857094</v>
+      </c>
+      <c r="CS45" s="2">
+        <v>806.22857142857197</v>
+      </c>
+      <c r="CT45" s="2">
+        <v>809.22857142857197</v>
+      </c>
+      <c r="CU45" s="2">
+        <v>919.22857142857299</v>
+      </c>
+      <c r="CV45" s="2">
+        <v>1311.2285714285699</v>
+      </c>
+      <c r="CW45" s="2">
+        <v>1528.2285714285699</v>
+      </c>
+      <c r="CX45" s="2">
+        <v>1680.2285714285699</v>
+      </c>
+      <c r="CY45" s="2">
+        <v>2345.2285714285699</v>
+      </c>
+      <c r="CZ45" s="2">
+        <v>2435.2285714285699</v>
+      </c>
+      <c r="DA45" s="2">
+        <v>2483.2285714285699</v>
+      </c>
+      <c r="DB45" s="2">
+        <v>3826.2285714285699</v>
+      </c>
+      <c r="DC45" s="2">
+        <v>2737.2285714285699</v>
+      </c>
+      <c r="DD45" s="2">
+        <v>779.22857142857299</v>
+      </c>
+      <c r="DE45" s="2">
+        <v>382.22857142857202</v>
+      </c>
+      <c r="DF45" s="2">
+        <v>271.22857142857202</v>
+      </c>
+      <c r="DG45" s="2">
+        <v>235.228571428572</v>
+      </c>
+      <c r="DH45" s="2">
+        <v>230.228571428572</v>
+      </c>
+    </row>
+    <row r="46" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR46" s="2">
+        <v>218</v>
+      </c>
+      <c r="CS46" s="2">
+        <v>204</v>
+      </c>
+      <c r="CT46" s="2">
+        <v>206</v>
+      </c>
+      <c r="CU46" s="2">
+        <v>215</v>
+      </c>
+      <c r="CV46" s="2">
+        <v>214</v>
+      </c>
+      <c r="CW46" s="2">
+        <v>235</v>
+      </c>
+      <c r="CX46" s="2">
+        <v>268</v>
+      </c>
+      <c r="CY46" s="2">
+        <v>292</v>
+      </c>
+      <c r="CZ46" s="2">
+        <v>287</v>
+      </c>
+      <c r="DA46" s="2">
+        <v>299</v>
+      </c>
+      <c r="DB46" s="2">
+        <v>306</v>
+      </c>
+      <c r="DC46" s="2">
+        <v>280</v>
+      </c>
+      <c r="DD46" s="2">
+        <v>200</v>
+      </c>
+      <c r="DE46" s="2">
+        <v>193</v>
+      </c>
+      <c r="DF46" s="2">
+        <v>222</v>
+      </c>
+      <c r="DG46" s="2">
+        <v>236</v>
+      </c>
+      <c r="DH46" s="2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR47" s="2">
+        <v>94.514285714285506</v>
+      </c>
+      <c r="CS47" s="2">
+        <v>111.51428571428499</v>
+      </c>
+      <c r="CT47" s="2">
+        <v>157.51428571428599</v>
+      </c>
+      <c r="CU47" s="2">
+        <v>243.51428571428599</v>
+      </c>
+      <c r="CV47" s="2">
+        <v>576.51428571428505</v>
+      </c>
+      <c r="CW47" s="2">
+        <v>825.51428571428596</v>
+      </c>
+      <c r="CX47" s="2">
+        <v>995.51428571428596</v>
+      </c>
+      <c r="CY47" s="2">
+        <v>1331.5142857142901</v>
+      </c>
+      <c r="CZ47" s="2">
+        <v>1517.51428571428</v>
+      </c>
+      <c r="DA47" s="2">
+        <v>1635.5142857142901</v>
+      </c>
+      <c r="DB47" s="2">
+        <v>1931.5142857142901</v>
+      </c>
+      <c r="DC47" s="2">
+        <v>1158.5142857142901</v>
+      </c>
+      <c r="DD47" s="2">
+        <v>157.51428571428599</v>
+      </c>
+      <c r="DE47" s="2">
+        <v>70.514285714285805</v>
+      </c>
+      <c r="DF47" s="2">
+        <v>41.514285714285798</v>
+      </c>
+      <c r="DG47" s="2">
+        <v>30.514285714285698</v>
+      </c>
+      <c r="DH47" s="2">
+        <v>-44.485714285714501</v>
+      </c>
+    </row>
+    <row r="48" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR48" s="2">
+        <v>1483.51428571428</v>
+      </c>
+      <c r="CS48" s="2">
+        <v>1401.51428571428</v>
+      </c>
+      <c r="CT48" s="2">
+        <v>1427.5142857142901</v>
+      </c>
+      <c r="CU48" s="2">
+        <v>1969.5142857142901</v>
+      </c>
+      <c r="CV48" s="2">
+        <v>1280.51428571428</v>
+      </c>
+      <c r="CW48" s="2">
+        <v>1347.5142857142901</v>
+      </c>
+      <c r="CX48" s="2">
+        <v>1245.5142857142901</v>
+      </c>
+      <c r="CY48" s="2">
+        <v>1913.51428571428</v>
+      </c>
+      <c r="CZ48" s="2">
+        <v>2036.51428571428</v>
+      </c>
+      <c r="DA48" s="2">
+        <v>2306.51428571428</v>
+      </c>
+      <c r="DB48" s="2">
+        <v>2446.51428571428</v>
+      </c>
+      <c r="DC48" s="2">
+        <v>1749.5142857142901</v>
+      </c>
+      <c r="DD48" s="2">
+        <v>1486.5142857142901</v>
+      </c>
+      <c r="DE48" s="2">
+        <v>877.51428571428505</v>
+      </c>
+      <c r="DF48" s="2">
+        <v>724.51428571428505</v>
+      </c>
+      <c r="DG48" s="2">
+        <v>707.51428571428596</v>
+      </c>
+      <c r="DH48" s="2">
+        <v>697.51428571428596</v>
+      </c>
+    </row>
+    <row r="49" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR49" s="2">
+        <v>83.257142857142696</v>
+      </c>
+      <c r="CS49" s="2">
+        <v>162.25714285714301</v>
+      </c>
+      <c r="CT49" s="2">
+        <v>115.25714285714299</v>
+      </c>
+      <c r="CU49" s="2">
+        <v>205.25714285714301</v>
+      </c>
+      <c r="CV49" s="2">
+        <v>258.25714285714298</v>
+      </c>
+      <c r="CW49" s="2">
+        <v>274.25714285714298</v>
+      </c>
+      <c r="CX49" s="2">
+        <v>413.25714285714298</v>
+      </c>
+      <c r="CY49" s="2">
+        <v>1018.25714285714</v>
+      </c>
+      <c r="CZ49" s="2">
+        <v>785.25714285714196</v>
+      </c>
+      <c r="DA49" s="2">
+        <v>1096.25714285714</v>
+      </c>
+      <c r="DB49" s="2">
+        <v>1061.25714285714</v>
+      </c>
+      <c r="DC49" s="2">
+        <v>587.25714285714298</v>
+      </c>
+      <c r="DD49" s="2">
+        <v>25.257142857143201</v>
+      </c>
+      <c r="DE49" s="2">
+        <v>1.2571428571429799</v>
+      </c>
+      <c r="DF49" s="2">
+        <v>-9.7428571428570905</v>
+      </c>
+      <c r="DG49" s="2">
+        <v>-2.7428571428569599</v>
+      </c>
+      <c r="DH49" s="2">
+        <v>3.2571428571430099</v>
+      </c>
+    </row>
+    <row r="50" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR50" s="2">
+        <v>238.74285714285699</v>
+      </c>
+      <c r="CS50" s="2">
+        <v>261.74285714285702</v>
+      </c>
+      <c r="CT50" s="2">
+        <v>216.74285714285699</v>
+      </c>
+      <c r="CU50" s="2">
+        <v>266.74285714285702</v>
+      </c>
+      <c r="CV50" s="2">
+        <v>230.74285714285699</v>
+      </c>
+      <c r="CW50" s="2">
+        <v>250.74285714285699</v>
+      </c>
+      <c r="CX50" s="2">
+        <v>336.74285714285702</v>
+      </c>
+      <c r="CY50" s="2">
+        <v>363.74285714285702</v>
+      </c>
+      <c r="CZ50" s="2">
+        <v>325.74285714285702</v>
+      </c>
+      <c r="DA50" s="2">
+        <v>338.74285714285702</v>
+      </c>
+      <c r="DB50" s="2">
+        <v>245.74285714285699</v>
+      </c>
+      <c r="DC50" s="2">
+        <v>160.74285714285699</v>
+      </c>
+      <c r="DD50" s="2">
+        <v>118.74285714285701</v>
+      </c>
+      <c r="DE50" s="2">
+        <v>119.74285714285701</v>
+      </c>
+      <c r="DF50" s="2">
+        <v>116.74285714285701</v>
+      </c>
+      <c r="DG50" s="2">
+        <v>117.74285714285701</v>
+      </c>
+      <c r="DH50" s="2">
+        <v>115.74285714285701</v>
+      </c>
+    </row>
+    <row r="51" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR51" s="2">
+        <v>93.799999999999898</v>
+      </c>
+      <c r="CS51" s="2">
+        <v>85.8</v>
+      </c>
+      <c r="CT51" s="2">
+        <v>60.8</v>
+      </c>
+      <c r="CU51" s="2">
+        <v>102.8</v>
+      </c>
+      <c r="CV51" s="2">
+        <v>104.8</v>
+      </c>
+      <c r="CW51" s="2">
+        <v>142.80000000000001</v>
+      </c>
+      <c r="CX51" s="2">
+        <v>155.80000000000001</v>
+      </c>
+      <c r="CY51" s="2">
+        <v>146.80000000000001</v>
+      </c>
+      <c r="CZ51" s="2">
+        <v>117.8</v>
+      </c>
+      <c r="DA51" s="2">
+        <v>123.8</v>
+      </c>
+      <c r="DB51" s="2">
+        <v>223.8</v>
+      </c>
+      <c r="DC51" s="2">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="DD51" s="2">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="DE51" s="2">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="DF51" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="DG51" s="2">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="DH51" s="2">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="52" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR52" s="2">
+        <v>245.542857142857</v>
+      </c>
+      <c r="CS52" s="2">
+        <v>239.542857142857</v>
+      </c>
+      <c r="CT52" s="2">
+        <v>237.542857142857</v>
+      </c>
+      <c r="CU52" s="2">
+        <v>262.54285714285697</v>
+      </c>
+      <c r="CV52" s="2">
+        <v>344.54285714285697</v>
+      </c>
+      <c r="CW52" s="2">
+        <v>410.54285714285697</v>
+      </c>
+      <c r="CX52" s="2">
+        <v>503.54285714285697</v>
+      </c>
+      <c r="CY52" s="2">
+        <v>732.54285714285595</v>
+      </c>
+      <c r="CZ52" s="2">
+        <v>853.54285714285595</v>
+      </c>
+      <c r="DA52" s="2">
+        <v>968.54285714285697</v>
+      </c>
+      <c r="DB52" s="2">
+        <v>1411.5428571428599</v>
+      </c>
+      <c r="DC52" s="2">
+        <v>728.54285714285697</v>
+      </c>
+      <c r="DD52" s="2">
+        <v>81.542857142857201</v>
+      </c>
+      <c r="DE52" s="2">
+        <v>97.542857142856803</v>
+      </c>
+      <c r="DF52" s="2">
+        <v>80.542857142856803</v>
+      </c>
+      <c r="DG52" s="2">
+        <v>62.542857142856903</v>
+      </c>
+      <c r="DH52" s="2">
+        <v>102.542857142857</v>
+      </c>
+    </row>
+    <row r="53" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR53" s="2">
+        <v>-22.1714285714284</v>
+      </c>
+      <c r="CS53" s="2">
+        <v>-18.171428571428599</v>
+      </c>
+      <c r="CT53" s="2">
+        <v>-18.171428571428699</v>
+      </c>
+      <c r="CU53" s="2">
+        <v>-33.1714285714285</v>
+      </c>
+      <c r="CV53" s="2">
+        <v>-31.171428571428301</v>
+      </c>
+      <c r="CW53" s="2">
+        <v>-36.171428571428301</v>
+      </c>
+      <c r="CX53" s="2">
+        <v>-28.171428571428699</v>
+      </c>
+      <c r="CY53" s="2">
+        <v>-23.1714285714285</v>
+      </c>
+      <c r="CZ53" s="2">
+        <v>-35.171428571428301</v>
+      </c>
+      <c r="DA53" s="2">
+        <v>-37.171428571428301</v>
+      </c>
+      <c r="DB53" s="2">
+        <v>-34.171428571428301</v>
+      </c>
+      <c r="DC53" s="2">
+        <v>-32.1714285714285</v>
+      </c>
+      <c r="DD53" s="2">
+        <v>-24.171428571428599</v>
+      </c>
+      <c r="DE53" s="2">
+        <v>-30.1714285714285</v>
+      </c>
+      <c r="DF53" s="2">
+        <v>-30.171428571428201</v>
+      </c>
+      <c r="DG53" s="2">
+        <v>-28.171428571428599</v>
+      </c>
+      <c r="DH53" s="2">
+        <v>-31.1714285714285</v>
+      </c>
+    </row>
+    <row r="54" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR54" s="2">
+        <v>457.74285714285702</v>
+      </c>
+      <c r="CS54" s="2">
+        <v>442.74285714285702</v>
+      </c>
+      <c r="CT54" s="2">
+        <v>425.74285714285702</v>
+      </c>
+      <c r="CU54" s="2">
+        <v>560.74285714285702</v>
+      </c>
+      <c r="CV54" s="2">
+        <v>520.74285714285702</v>
+      </c>
+      <c r="CW54" s="2">
+        <v>508.74285714285702</v>
+      </c>
+      <c r="CX54" s="2">
+        <v>538.74285714285702</v>
+      </c>
+      <c r="CY54" s="2">
+        <v>589.74285714285702</v>
+      </c>
+      <c r="CZ54" s="2">
+        <v>593.74285714285702</v>
+      </c>
+      <c r="DA54" s="2">
+        <v>532.74285714285702</v>
+      </c>
+      <c r="DB54" s="2">
+        <v>460.74285714285702</v>
+      </c>
+      <c r="DC54" s="2">
+        <v>289.74285714285702</v>
+      </c>
+      <c r="DD54" s="2">
+        <v>215.74285714285699</v>
+      </c>
+      <c r="DE54" s="2">
+        <v>177.74285714285699</v>
+      </c>
+      <c r="DF54" s="2">
+        <v>153.74285714285699</v>
+      </c>
+      <c r="DG54" s="2">
+        <v>156.74285714285699</v>
+      </c>
+      <c r="DH54" s="2">
+        <v>172.74285714285699</v>
+      </c>
+    </row>
+    <row r="55" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR55" s="2">
+        <v>244.37142857142899</v>
+      </c>
+      <c r="CS55" s="2">
+        <v>316.37142857142902</v>
+      </c>
+      <c r="CT55" s="2">
+        <v>274.37142857142902</v>
+      </c>
+      <c r="CU55" s="2">
+        <v>314.37142857142902</v>
+      </c>
+      <c r="CV55" s="2">
+        <v>401.37142857142902</v>
+      </c>
+      <c r="CW55" s="2">
+        <v>437.37142857142902</v>
+      </c>
+      <c r="CX55" s="2">
+        <v>659.37142857142896</v>
+      </c>
+      <c r="CY55" s="2">
+        <v>725.37142857142896</v>
+      </c>
+      <c r="CZ55" s="2">
+        <v>889.37142857142896</v>
+      </c>
+      <c r="DA55" s="2">
+        <v>881.37142857142896</v>
+      </c>
+      <c r="DB55" s="2">
+        <v>1077.37142857143</v>
+      </c>
+      <c r="DC55" s="2">
+        <v>594.37142857142896</v>
+      </c>
+      <c r="DD55" s="2">
+        <v>188.37142857142899</v>
+      </c>
+      <c r="DE55" s="2">
+        <v>181.37142857142899</v>
+      </c>
+      <c r="DF55" s="2">
+        <v>179.37142857142899</v>
+      </c>
+      <c r="DG55" s="2">
+        <v>205.37142857142899</v>
+      </c>
+      <c r="DH55" s="2">
+        <v>243.37142857142899</v>
+      </c>
+    </row>
+    <row r="56" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR56" s="2">
+        <v>-19.571428571428498</v>
+      </c>
+      <c r="CS56" s="2">
+        <v>84.428571428571402</v>
+      </c>
+      <c r="CT56" s="2">
+        <v>104.428571428572</v>
+      </c>
+      <c r="CU56" s="2">
+        <v>93.428571428571402</v>
+      </c>
+      <c r="CV56" s="2">
+        <v>55.428571428571402</v>
+      </c>
+      <c r="CW56" s="2">
+        <v>27.428571428571399</v>
+      </c>
+      <c r="CX56" s="2">
+        <v>35.428571428571402</v>
+      </c>
+      <c r="CY56" s="2">
+        <v>48.428571428571402</v>
+      </c>
+      <c r="CZ56" s="2">
+        <v>58.428571428571402</v>
+      </c>
+      <c r="DA56" s="2">
+        <v>34.428571428571402</v>
+      </c>
+      <c r="DB56" s="2">
+        <v>240.42857142857099</v>
+      </c>
+      <c r="DC56" s="2">
+        <v>180.42857142857201</v>
+      </c>
+      <c r="DD56" s="2">
+        <v>54.428571428571402</v>
+      </c>
+      <c r="DE56" s="2">
+        <v>32.428571428571402</v>
+      </c>
+      <c r="DF56" s="2">
+        <v>25.428571428571399</v>
+      </c>
+      <c r="DG56" s="2">
+        <v>-1.5714285714285801</v>
+      </c>
+      <c r="DH56" s="2">
+        <v>-9.5714285714285605</v>
+      </c>
+    </row>
+    <row r="57" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR57" s="2">
+        <v>123.028571428571</v>
+      </c>
+      <c r="CS57" s="2">
+        <v>154.02857142857101</v>
+      </c>
+      <c r="CT57" s="2">
+        <v>202.02857142857201</v>
+      </c>
+      <c r="CU57" s="2">
+        <v>268.02857142857198</v>
+      </c>
+      <c r="CV57" s="2">
+        <v>324.02857142857101</v>
+      </c>
+      <c r="CW57" s="2">
+        <v>340.02857142857101</v>
+      </c>
+      <c r="CX57" s="2">
+        <v>433.02857142857198</v>
+      </c>
+      <c r="CY57" s="2">
+        <v>684.02857142857101</v>
+      </c>
+      <c r="CZ57" s="2">
+        <v>727.02857142857101</v>
+      </c>
+      <c r="DA57" s="2">
+        <v>699.02857142857204</v>
+      </c>
+      <c r="DB57" s="2">
+        <v>804.02857142857101</v>
+      </c>
+      <c r="DC57" s="2">
+        <v>629.02857142857204</v>
+      </c>
+      <c r="DD57" s="2">
+        <v>130.02857142857101</v>
+      </c>
+      <c r="DE57" s="2">
+        <v>89.028571428571396</v>
+      </c>
+      <c r="DF57" s="2">
+        <v>75.028571428571297</v>
+      </c>
+      <c r="DG57" s="2">
+        <v>67.028571428571297</v>
+      </c>
+      <c r="DH57" s="2">
+        <v>85.028571428571396</v>
+      </c>
+    </row>
+    <row r="58" spans="96:112" x14ac:dyDescent="0.25">
+      <c r="CR58" s="2">
+        <v>69.171428571428507</v>
+      </c>
+      <c r="CS58" s="2">
+        <v>55.1714285714285</v>
+      </c>
+      <c r="CT58" s="2">
+        <v>74.171428571428706</v>
+      </c>
+      <c r="CU58" s="2">
+        <v>98.171428571428606</v>
+      </c>
+      <c r="CV58" s="2">
+        <v>79.171428571428507</v>
+      </c>
+      <c r="CW58" s="2">
+        <v>84.171428571428507</v>
+      </c>
+      <c r="CX58" s="2">
+        <v>107.171428571429</v>
+      </c>
+      <c r="CY58" s="2">
+        <v>144.17142857142801</v>
+      </c>
+      <c r="CZ58" s="2">
+        <v>135.17142857142801</v>
+      </c>
+      <c r="DA58" s="2">
+        <v>116.171428571429</v>
+      </c>
+      <c r="DB58" s="2">
+        <v>86.171428571428507</v>
+      </c>
+      <c r="DC58" s="2">
+        <v>36.171428571428599</v>
+      </c>
+      <c r="DD58" s="2">
+        <v>9.1714285714285495</v>
+      </c>
+      <c r="DE58" s="2">
+        <v>7.1714285714285602</v>
+      </c>
+      <c r="DF58" s="2">
+        <v>4.1714285714285397</v>
+      </c>
+      <c r="DG58" s="2">
+        <v>4.1714285714285504</v>
+      </c>
+      <c r="DH58" s="2">
+        <v>2.1714285714285602</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>